<commit_message>
bal mss for pr 4e09026b3efe18db6c260ee07b5cbe018efb892f
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitionerrole.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitionerrole.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T09:36:20+00:00</t>
+    <t>2024-11-13T09:52:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1396,8 +1396,8 @@
     <t>Often practitioners have a dedicated line for each location (or service) that they work at, and need to be able to define separate contact details for each of these.</t>
   </si>
   <si>
-    <t xml:space="preserve">profile:$this.resolve()}
-</t>
+    <t>pattern:system}
+exists:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type')}</t>
   </si>
   <si>
     <t>closed</t>
@@ -2361,7 +2361,7 @@
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="105.0546875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="89.67578125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>